<commit_message>
add editor for excel
</commit_message>
<xml_diff>
--- a/Assets/Test/Test3.xlsx
+++ b/Assets/Test/Test3.xlsx
@@ -16,10 +16,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -383,40 +379,957 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:11">
       <c r="A1">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="B1">
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="C1">
-        <v>33</v>
+        <v>3</v>
       </c>
       <c r="D1">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>4</v>
+      </c>
+      <c r="E1">
+        <v>5</v>
+      </c>
+      <c r="F1">
+        <v>6</v>
+      </c>
+      <c r="G1">
+        <v>7</v>
+      </c>
+      <c r="H1">
+        <v>8</v>
+      </c>
+      <c r="I1">
+        <v>9</v>
+      </c>
+      <c r="J1">
+        <v>10</v>
+      </c>
+      <c r="K1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="C2">
-        <v>33</v>
+        <v>3</v>
       </c>
       <c r="D2">
-        <v>33</v>
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <v>6</v>
+      </c>
+      <c r="G2">
+        <v>7</v>
+      </c>
+      <c r="H2">
+        <v>8</v>
+      </c>
+      <c r="I2">
+        <v>9</v>
+      </c>
+      <c r="J2">
+        <v>10</v>
+      </c>
+      <c r="K2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>6</v>
+      </c>
+      <c r="G3">
+        <v>7</v>
+      </c>
+      <c r="H3">
+        <v>8</v>
+      </c>
+      <c r="I3">
+        <v>9</v>
+      </c>
+      <c r="J3">
+        <v>10</v>
+      </c>
+      <c r="K3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>6</v>
+      </c>
+      <c r="G4">
+        <v>7</v>
+      </c>
+      <c r="H4">
+        <v>8</v>
+      </c>
+      <c r="I4">
+        <v>9</v>
+      </c>
+      <c r="J4">
+        <v>10</v>
+      </c>
+      <c r="K4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>6</v>
+      </c>
+      <c r="G5">
+        <v>7</v>
+      </c>
+      <c r="H5">
+        <v>8</v>
+      </c>
+      <c r="I5">
+        <v>9</v>
+      </c>
+      <c r="J5">
+        <v>10</v>
+      </c>
+      <c r="K5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>6</v>
+      </c>
+      <c r="G6">
+        <v>7</v>
+      </c>
+      <c r="H6">
+        <v>8</v>
+      </c>
+      <c r="I6">
+        <v>9</v>
+      </c>
+      <c r="J6">
+        <v>10</v>
+      </c>
+      <c r="K6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>6</v>
+      </c>
+      <c r="G7">
+        <v>7</v>
+      </c>
+      <c r="H7">
+        <v>8</v>
+      </c>
+      <c r="I7">
+        <v>9</v>
+      </c>
+      <c r="J7">
+        <v>10</v>
+      </c>
+      <c r="K7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8">
+        <v>6</v>
+      </c>
+      <c r="G8">
+        <v>7</v>
+      </c>
+      <c r="H8">
+        <v>8</v>
+      </c>
+      <c r="I8">
+        <v>9</v>
+      </c>
+      <c r="J8">
+        <v>10</v>
+      </c>
+      <c r="K8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="F9">
+        <v>6</v>
+      </c>
+      <c r="G9">
+        <v>7</v>
+      </c>
+      <c r="H9">
+        <v>8</v>
+      </c>
+      <c r="I9">
+        <v>9</v>
+      </c>
+      <c r="J9">
+        <v>10</v>
+      </c>
+      <c r="K9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+      <c r="F10">
+        <v>6</v>
+      </c>
+      <c r="G10">
+        <v>7</v>
+      </c>
+      <c r="H10">
+        <v>8</v>
+      </c>
+      <c r="I10">
+        <v>9</v>
+      </c>
+      <c r="J10">
+        <v>10</v>
+      </c>
+      <c r="K10">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>5</v>
+      </c>
+      <c r="F11">
+        <v>6</v>
+      </c>
+      <c r="G11">
+        <v>7</v>
+      </c>
+      <c r="H11">
+        <v>8</v>
+      </c>
+      <c r="I11">
+        <v>9</v>
+      </c>
+      <c r="J11">
+        <v>10</v>
+      </c>
+      <c r="K11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
+      <c r="E12">
+        <v>5</v>
+      </c>
+      <c r="F12">
+        <v>6</v>
+      </c>
+      <c r="G12">
+        <v>7</v>
+      </c>
+      <c r="H12">
+        <v>8</v>
+      </c>
+      <c r="I12">
+        <v>9</v>
+      </c>
+      <c r="J12">
+        <v>10</v>
+      </c>
+      <c r="K12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="E13">
+        <v>5</v>
+      </c>
+      <c r="F13">
+        <v>6</v>
+      </c>
+      <c r="G13">
+        <v>7</v>
+      </c>
+      <c r="H13">
+        <v>8</v>
+      </c>
+      <c r="I13">
+        <v>9</v>
+      </c>
+      <c r="J13">
+        <v>10</v>
+      </c>
+      <c r="K13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="E14">
+        <v>5</v>
+      </c>
+      <c r="F14">
+        <v>6</v>
+      </c>
+      <c r="G14">
+        <v>7</v>
+      </c>
+      <c r="H14">
+        <v>8</v>
+      </c>
+      <c r="I14">
+        <v>9</v>
+      </c>
+      <c r="J14">
+        <v>10</v>
+      </c>
+      <c r="K14">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+      <c r="E15">
+        <v>5</v>
+      </c>
+      <c r="F15">
+        <v>6</v>
+      </c>
+      <c r="G15">
+        <v>7</v>
+      </c>
+      <c r="H15">
+        <v>8</v>
+      </c>
+      <c r="I15">
+        <v>9</v>
+      </c>
+      <c r="J15">
+        <v>10</v>
+      </c>
+      <c r="K15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+      <c r="E16">
+        <v>5</v>
+      </c>
+      <c r="F16">
+        <v>6</v>
+      </c>
+      <c r="G16">
+        <v>7</v>
+      </c>
+      <c r="H16">
+        <v>8</v>
+      </c>
+      <c r="I16">
+        <v>9</v>
+      </c>
+      <c r="J16">
+        <v>10</v>
+      </c>
+      <c r="K16">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17">
+        <v>4</v>
+      </c>
+      <c r="E17">
+        <v>5</v>
+      </c>
+      <c r="F17">
+        <v>6</v>
+      </c>
+      <c r="G17">
+        <v>7</v>
+      </c>
+      <c r="H17">
+        <v>8</v>
+      </c>
+      <c r="I17">
+        <v>9</v>
+      </c>
+      <c r="J17">
+        <v>10</v>
+      </c>
+      <c r="K17">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>4</v>
+      </c>
+      <c r="E18">
+        <v>5</v>
+      </c>
+      <c r="F18">
+        <v>6</v>
+      </c>
+      <c r="G18">
+        <v>7</v>
+      </c>
+      <c r="H18">
+        <v>8</v>
+      </c>
+      <c r="I18">
+        <v>9</v>
+      </c>
+      <c r="J18">
+        <v>10</v>
+      </c>
+      <c r="K18">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+      <c r="D19">
+        <v>4</v>
+      </c>
+      <c r="E19">
+        <v>5</v>
+      </c>
+      <c r="F19">
+        <v>6</v>
+      </c>
+      <c r="G19">
+        <v>7</v>
+      </c>
+      <c r="H19">
+        <v>8</v>
+      </c>
+      <c r="I19">
+        <v>9</v>
+      </c>
+      <c r="J19">
+        <v>10</v>
+      </c>
+      <c r="K19">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <v>4</v>
+      </c>
+      <c r="E20">
+        <v>5</v>
+      </c>
+      <c r="F20">
+        <v>6</v>
+      </c>
+      <c r="G20">
+        <v>7</v>
+      </c>
+      <c r="H20">
+        <v>8</v>
+      </c>
+      <c r="I20">
+        <v>9</v>
+      </c>
+      <c r="J20">
+        <v>10</v>
+      </c>
+      <c r="K20">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="D21">
+        <v>4</v>
+      </c>
+      <c r="E21">
+        <v>5</v>
+      </c>
+      <c r="F21">
+        <v>6</v>
+      </c>
+      <c r="G21">
+        <v>7</v>
+      </c>
+      <c r="H21">
+        <v>8</v>
+      </c>
+      <c r="I21">
+        <v>9</v>
+      </c>
+      <c r="J21">
+        <v>10</v>
+      </c>
+      <c r="K21">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22">
+        <v>4</v>
+      </c>
+      <c r="E22">
+        <v>5</v>
+      </c>
+      <c r="F22">
+        <v>6</v>
+      </c>
+      <c r="G22">
+        <v>7</v>
+      </c>
+      <c r="H22">
+        <v>8</v>
+      </c>
+      <c r="I22">
+        <v>9</v>
+      </c>
+      <c r="J22">
+        <v>10</v>
+      </c>
+      <c r="K22">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23">
+        <v>4</v>
+      </c>
+      <c r="E23">
+        <v>5</v>
+      </c>
+      <c r="F23">
+        <v>6</v>
+      </c>
+      <c r="G23">
+        <v>7</v>
+      </c>
+      <c r="H23">
+        <v>8</v>
+      </c>
+      <c r="I23">
+        <v>9</v>
+      </c>
+      <c r="J23">
+        <v>10</v>
+      </c>
+      <c r="K23">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24">
+        <v>4</v>
+      </c>
+      <c r="E24">
+        <v>5</v>
+      </c>
+      <c r="F24">
+        <v>6</v>
+      </c>
+      <c r="G24">
+        <v>7</v>
+      </c>
+      <c r="H24">
+        <v>8</v>
+      </c>
+      <c r="I24">
+        <v>9</v>
+      </c>
+      <c r="J24">
+        <v>10</v>
+      </c>
+      <c r="K24">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25">
+        <v>4</v>
+      </c>
+      <c r="E25">
+        <v>5</v>
+      </c>
+      <c r="F25">
+        <v>6</v>
+      </c>
+      <c r="G25">
+        <v>7</v>
+      </c>
+      <c r="H25">
+        <v>8</v>
+      </c>
+      <c r="I25">
+        <v>9</v>
+      </c>
+      <c r="J25">
+        <v>10</v>
+      </c>
+      <c r="K25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+      <c r="D26">
+        <v>4</v>
+      </c>
+      <c r="E26">
+        <v>5</v>
+      </c>
+      <c r="F26">
+        <v>6</v>
+      </c>
+      <c r="G26">
+        <v>7</v>
+      </c>
+      <c r="H26">
+        <v>8</v>
+      </c>
+      <c r="I26">
+        <v>9</v>
+      </c>
+      <c r="J26">
+        <v>10</v>
+      </c>
+      <c r="K26">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27">
+        <v>4</v>
+      </c>
+      <c r="E27">
+        <v>5</v>
+      </c>
+      <c r="F27">
+        <v>6</v>
+      </c>
+      <c r="G27">
+        <v>7</v>
+      </c>
+      <c r="H27">
+        <v>8</v>
+      </c>
+      <c r="I27">
+        <v>9</v>
+      </c>
+      <c r="J27">
+        <v>10</v>
+      </c>
+      <c r="K27">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
* add new cell type "popup"
</commit_message>
<xml_diff>
--- a/Assets/Test/Test3.xlsx
+++ b/Assets/Test/Test3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="0" windowWidth="25600" windowHeight="15160" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="0" windowWidth="25600" windowHeight="15160"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="17">
   <si>
     <t>ID</t>
   </si>
@@ -35,9 +35,6 @@
   </si>
   <si>
     <t>1111</t>
-  </si>
-  <si>
-    <t>3</t>
   </si>
   <si>
     <t>4</t>
@@ -71,6 +68,9 @@
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>Type</t>
   </si>
 </sst>
 </file>
@@ -112,17 +112,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -454,8 +458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:K7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -468,7 +472,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -503,7 +507,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
@@ -537,32 +541,32 @@
       <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
+      <c r="C3">
+        <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -570,34 +574,34 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
+        <v>13</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -605,34 +609,34 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -640,34 +644,34 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -675,34 +679,34 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -710,34 +714,34 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
+        <v>13</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -745,34 +749,34 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
+        <v>13</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -780,34 +784,34 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
+        <v>13</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -815,34 +819,34 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" t="s">
-        <v>5</v>
+        <v>13</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -850,34 +854,34 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" t="s">
-        <v>5</v>
+        <v>13</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -885,34 +889,34 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" t="s">
-        <v>5</v>
+        <v>13</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -920,34 +924,34 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" t="s">
-        <v>5</v>
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -955,34 +959,34 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" t="s">
-        <v>5</v>
+        <v>13</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -990,34 +994,34 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" t="s">
-        <v>5</v>
+        <v>13</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -1025,34 +1029,34 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" t="s">
-        <v>5</v>
+        <v>13</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1060,34 +1064,34 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" t="s">
-        <v>5</v>
+        <v>13</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1095,34 +1099,34 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" t="s">
-        <v>5</v>
+        <v>13</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1130,34 +1134,34 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" t="s">
-        <v>5</v>
+        <v>13</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -1165,34 +1169,34 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" t="s">
-        <v>5</v>
+        <v>13</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -1200,34 +1204,34 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" t="s">
-        <v>5</v>
+        <v>13</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E22" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -1235,34 +1239,34 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" t="s">
-        <v>5</v>
+        <v>13</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E23" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G23" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K23" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -1270,34 +1274,34 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24" t="s">
-        <v>5</v>
+        <v>13</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -1305,34 +1309,34 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>14</v>
-      </c>
-      <c r="C25" t="s">
-        <v>5</v>
+        <v>13</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -1340,34 +1344,34 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>14</v>
-      </c>
-      <c r="C26" t="s">
-        <v>5</v>
+        <v>13</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E26" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G26" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -1375,214 +1379,213 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27" t="s">
-        <v>5</v>
+        <v>13</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E27" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J27" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:11">
       <c r="A29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:11">
       <c r="A30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:11">
       <c r="A31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:11">
       <c r="A32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1595,8 +1598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1609,7 +1612,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -1644,7 +1647,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
@@ -1679,7 +1682,7 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -1714,7 +1717,7 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -1749,7 +1752,7 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1784,7 +1787,7 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1819,7 +1822,7 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1848,6 +1851,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>